<commit_message>
modify template test data
</commit_message>
<xml_diff>
--- a/data/template/TEMPLATE_TEST_DATA.xlsx
+++ b/data/template/TEMPLATE_TEST_DATA.xlsx
@@ -144,9 +144,6 @@
     <t>my.vu@c-mg.com</t>
   </si>
   <si>
-    <t>GOO(oil)</t>
-  </si>
-  <si>
     <t>tester</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>vum003</t>
+  </si>
+  <si>
+    <t>GPO</t>
   </si>
 </sst>
 </file>
@@ -744,8 +744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK235"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -997,7 +997,7 @@
     </row>
     <row r="5" spans="1:37">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" s="2">
         <v>902</v>
@@ -1012,146 +1012,146 @@
         <v>41</v>
       </c>
       <c r="F5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="O5" s="13" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="P5" s="13" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="Q5" s="13" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:37">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2">
         <v>89820</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="F6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="K6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="N6" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="O6" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P6" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:37">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="2">
         <v>24687</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="E7" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="F7" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="H7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="K7" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="L7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="N7" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="O7" s="13" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="P7" s="13" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="Q7" s="13" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:37">

</xml_diff>